<commit_message>
thought we were working on this today, did not finish, push after class review
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tayjy\Documents\DA11\Excel\lookups-exercise-Jordan-D-Taylor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87DF7C63-C5CC-4FEF-9BAE-566AF0A6E42D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA3089FC-1C10-4619-BD8A-87032EC253E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="18450" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metro_budget" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="91">
   <si>
     <t>Department</t>
   </si>
@@ -304,6 +304,9 @@
   </si>
   <si>
     <t>Actual spending amount - budget amount for fiscal year 2019</t>
+  </si>
+  <si>
+    <t>Review</t>
   </si>
 </sst>
 </file>
@@ -1178,8 +1181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H62" sqref="H62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1261,12 +1264,12 @@
         <v>-15396420.870000005</v>
       </c>
       <c r="E2" s="5">
-        <f>IFERROR(D2/B2,"")</f>
+        <f>IFERROR(D2/B2,0)</f>
         <v>-4.3170750765267295E-2</v>
       </c>
       <c r="F2">
-        <f>IFERROR(_xlfn.RANK.EQ(E2,$E$2:$E$52),"")</f>
-        <v>35</v>
+        <f>RANK(E2,$E$2:$E$52,1)</f>
+        <v>14</v>
       </c>
       <c r="G2">
         <v>382685200</v>
@@ -1279,12 +1282,12 @@
         <v>-36344389.180000007</v>
       </c>
       <c r="J2" s="5">
-        <f>IFERROR(I2/G2,"")</f>
+        <f>IFERROR(I2/G2,0)</f>
         <v>-9.4972027086493035E-2</v>
       </c>
       <c r="K2">
-        <f>IFERROR(_xlfn.RANK.EQ(J2,$J$2:$J$52),"")</f>
-        <v>39</v>
+        <f>RANK(J2,$J$2:$J$52)</f>
+        <v>42</v>
       </c>
       <c r="L2">
         <v>376548600</v>
@@ -1297,12 +1300,12 @@
         <v>-21269107.770000994</v>
       </c>
       <c r="O2" s="5">
-        <f>IFERROR(N2/L2,"")</f>
+        <f>IFERROR(N2/L2,0)</f>
         <v>-5.6484362894991494E-2</v>
       </c>
       <c r="P2">
-        <f>IFERROR(_xlfn.RANK.EQ(O2,$O$2:$O$52),"")</f>
-        <v>35</v>
+        <f>_xlfn.RANK.EQ(O2,$O$2:$O$52)</f>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -1320,12 +1323,12 @@
         <v>-7585.4099999999744</v>
       </c>
       <c r="E3" s="5">
-        <f t="shared" ref="E3:E52" si="1">IFERROR(D3/B3,"")</f>
+        <f t="shared" ref="E3:E52" si="1">IFERROR(D3/B3,0)</f>
         <v>-2.3069981751824741E-2</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F52" si="2">IFERROR(_xlfn.RANK.EQ(E3,$E$2:$E$52),"")</f>
-        <v>27</v>
+        <f t="shared" ref="F3:F52" si="2">RANK(E3,$E$2:$E$52,1)</f>
+        <v>22</v>
       </c>
       <c r="G3">
         <v>334800</v>
@@ -1338,12 +1341,12 @@
         <v>-22366.290000001027</v>
       </c>
       <c r="J3" s="5">
-        <f t="shared" ref="J3:J52" si="4">IFERROR(I3/G3,"")</f>
+        <f t="shared" ref="J3:J52" si="4">IFERROR(I3/G3,0)</f>
         <v>-6.6804928315415249E-2</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K52" si="5">IFERROR(_xlfn.RANK.EQ(J3,$J$2:$J$52),"")</f>
-        <v>35</v>
+        <f t="shared" ref="K3:K52" si="5">RANK(J3,$J$2:$J$52)</f>
+        <v>38</v>
       </c>
       <c r="L3">
         <v>322700</v>
@@ -1356,12 +1359,12 @@
         <v>-436.96000000002095</v>
       </c>
       <c r="O3" s="5">
-        <f t="shared" ref="O3:O52" si="7">IFERROR(N3/L3,"")</f>
+        <f t="shared" ref="O3:O52" si="7">IFERROR(N3/L3,0)</f>
         <v>-1.3540749922529313E-3</v>
       </c>
       <c r="P3">
-        <f t="shared" ref="P3:P52" si="8">IFERROR(_xlfn.RANK.EQ(O3,$O$2:$O$52),"")</f>
-        <v>12</v>
+        <f t="shared" ref="P3:P52" si="8">_xlfn.RANK.EQ(O3,$O$2:$O$52)</f>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -1384,7 +1387,7 @@
       </c>
       <c r="F4">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="G4">
         <v>3652300</v>
@@ -1402,7 +1405,7 @@
       </c>
       <c r="K4">
         <f t="shared" si="5"/>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="L4">
         <v>3662400</v>
@@ -1420,7 +1423,7 @@
       </c>
       <c r="P4">
         <f t="shared" si="8"/>
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -1443,7 +1446,7 @@
       </c>
       <c r="F5">
         <f t="shared" si="2"/>
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="G5">
         <v>7968300</v>
@@ -1461,7 +1464,7 @@
       </c>
       <c r="K5">
         <f t="shared" si="5"/>
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="L5">
         <v>7759600</v>
@@ -1479,7 +1482,7 @@
       </c>
       <c r="P5">
         <f t="shared" si="8"/>
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -1502,7 +1505,7 @@
       </c>
       <c r="F6">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="G6">
         <v>428500</v>
@@ -1520,7 +1523,7 @@
       </c>
       <c r="K6">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="L6">
         <v>445200</v>
@@ -1538,7 +1541,7 @@
       </c>
       <c r="P6">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -1561,7 +1564,7 @@
       </c>
       <c r="F7">
         <f t="shared" si="2"/>
-        <v>47</v>
+        <v>2</v>
       </c>
       <c r="G7">
         <v>3390900</v>
@@ -1579,7 +1582,7 @@
       </c>
       <c r="K7">
         <f t="shared" si="5"/>
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="L7">
         <v>3345200</v>
@@ -1597,7 +1600,7 @@
       </c>
       <c r="P7">
         <f t="shared" si="8"/>
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -1620,7 +1623,7 @@
       </c>
       <c r="F8">
         <f t="shared" si="2"/>
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="G8">
         <v>1590700</v>
@@ -1638,7 +1641,7 @@
       </c>
       <c r="K8">
         <f t="shared" si="5"/>
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="L8">
         <v>1579300</v>
@@ -1656,7 +1659,7 @@
       </c>
       <c r="P8">
         <f t="shared" si="8"/>
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -1679,7 +1682,7 @@
       </c>
       <c r="F9">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="G9">
         <v>11073700</v>
@@ -1697,7 +1700,7 @@
       </c>
       <c r="K9">
         <f t="shared" si="5"/>
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="L9">
         <v>10790500</v>
@@ -1715,7 +1718,7 @@
       </c>
       <c r="P9">
         <f t="shared" si="8"/>
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -1738,7 +1741,7 @@
       </c>
       <c r="F10">
         <f t="shared" si="2"/>
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="G10">
         <v>495200</v>
@@ -1756,7 +1759,7 @@
       </c>
       <c r="K10">
         <f t="shared" si="5"/>
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="L10">
         <v>487500</v>
@@ -1774,7 +1777,7 @@
       </c>
       <c r="P10">
         <f t="shared" si="8"/>
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -1791,13 +1794,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E11" s="5" t="str">
+      <c r="E11" s="5">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F11" t="str">
+        <v>0</v>
+      </c>
+      <c r="F11">
         <f t="shared" si="2"/>
-        <v/>
+        <v>47</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -1809,13 +1812,13 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J11" s="5" t="str">
+      <c r="J11" s="5">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="K11" t="str">
+        <v>0</v>
+      </c>
+      <c r="K11">
         <f t="shared" si="5"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="L11">
         <v>375000</v>
@@ -1833,7 +1836,7 @@
       </c>
       <c r="P11">
         <f t="shared" si="8"/>
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -1856,7 +1859,7 @@
       </c>
       <c r="F12">
         <f t="shared" si="2"/>
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="G12">
         <v>4700400</v>
@@ -1874,7 +1877,7 @@
       </c>
       <c r="K12">
         <f t="shared" si="5"/>
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="L12">
         <v>4677800</v>
@@ -1892,7 +1895,7 @@
       </c>
       <c r="P12">
         <f t="shared" si="8"/>
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -1915,7 +1918,7 @@
       </c>
       <c r="F13">
         <f t="shared" si="2"/>
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="G13">
         <v>6223700</v>
@@ -1933,7 +1936,7 @@
       </c>
       <c r="K13">
         <f t="shared" si="5"/>
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="L13">
         <v>6207300</v>
@@ -1951,7 +1954,7 @@
       </c>
       <c r="P13">
         <f t="shared" si="8"/>
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -1974,7 +1977,7 @@
       </c>
       <c r="F14">
         <f t="shared" si="2"/>
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="G14">
         <v>530500</v>
@@ -1992,7 +1995,7 @@
       </c>
       <c r="K14">
         <f t="shared" si="5"/>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="L14">
         <v>526200</v>
@@ -2010,7 +2013,7 @@
       </c>
       <c r="P14">
         <f t="shared" si="8"/>
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -2033,7 +2036,7 @@
       </c>
       <c r="F15">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="G15">
         <v>184167800</v>
@@ -2051,7 +2054,7 @@
       </c>
       <c r="K15">
         <f t="shared" si="5"/>
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="L15">
         <v>188953500</v>
@@ -2069,7 +2072,7 @@
       </c>
       <c r="P15">
         <f t="shared" si="8"/>
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -2092,7 +2095,7 @@
       </c>
       <c r="F16">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="G16">
         <v>7352500</v>
@@ -2110,7 +2113,7 @@
       </c>
       <c r="K16">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L16">
         <v>7397200</v>
@@ -2128,7 +2131,7 @@
       </c>
       <c r="P16">
         <f t="shared" si="8"/>
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
@@ -2151,7 +2154,7 @@
       </c>
       <c r="F17">
         <f t="shared" si="2"/>
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="G17">
         <v>15309700</v>
@@ -2169,7 +2172,7 @@
       </c>
       <c r="K17">
         <f t="shared" si="5"/>
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="L17">
         <v>15311800</v>
@@ -2187,7 +2190,7 @@
       </c>
       <c r="P17">
         <f t="shared" si="8"/>
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -2210,7 +2213,7 @@
       </c>
       <c r="F18">
         <f t="shared" si="2"/>
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="G18">
         <v>2861000</v>
@@ -2228,7 +2231,7 @@
       </c>
       <c r="K18">
         <f t="shared" si="5"/>
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="L18">
         <v>2910600</v>
@@ -2246,7 +2249,7 @@
       </c>
       <c r="P18">
         <f t="shared" si="8"/>
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -2269,7 +2272,7 @@
       </c>
       <c r="F19">
         <f t="shared" si="2"/>
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="G19">
         <v>9713300</v>
@@ -2287,7 +2290,7 @@
       </c>
       <c r="K19">
         <f t="shared" si="5"/>
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="L19">
         <v>9343000</v>
@@ -2305,7 +2308,7 @@
       </c>
       <c r="P19">
         <f t="shared" si="8"/>
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
@@ -2323,12 +2326,12 @@
         <v>-1539.8400010019541</v>
       </c>
       <c r="E20" s="5">
-        <f>IFERROR(D20/B20,"")</f>
+        <f t="shared" si="1"/>
         <v>-1.2379538203300809E-5</v>
       </c>
       <c r="F20">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>46</v>
       </c>
       <c r="G20">
         <v>131849400</v>
@@ -2346,7 +2349,7 @@
       </c>
       <c r="K20">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L20">
         <v>130621400</v>
@@ -2364,7 +2367,7 @@
       </c>
       <c r="P20">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
@@ -2387,7 +2390,7 @@
       </c>
       <c r="F21">
         <f t="shared" si="2"/>
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="G21">
         <v>24497400</v>
@@ -2405,7 +2408,7 @@
       </c>
       <c r="K21">
         <f t="shared" si="5"/>
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="L21">
         <v>24323000</v>
@@ -2423,7 +2426,7 @@
       </c>
       <c r="P21">
         <f t="shared" si="8"/>
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -2446,7 +2449,7 @@
       </c>
       <c r="F22">
         <f t="shared" si="2"/>
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="G22">
         <v>11980700</v>
@@ -2464,7 +2467,7 @@
       </c>
       <c r="K22">
         <f t="shared" si="5"/>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="L22">
         <v>11935200</v>
@@ -2482,7 +2485,7 @@
       </c>
       <c r="P22">
         <f t="shared" si="8"/>
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -2505,7 +2508,7 @@
       </c>
       <c r="F23">
         <f t="shared" si="2"/>
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="G23">
         <v>22683800</v>
@@ -2523,7 +2526,7 @@
       </c>
       <c r="K23">
         <f t="shared" si="5"/>
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="L23">
         <v>23220300</v>
@@ -2541,7 +2544,7 @@
       </c>
       <c r="P23">
         <f t="shared" si="8"/>
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
@@ -2564,7 +2567,7 @@
       </c>
       <c r="F24">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="G24">
         <v>1112700</v>
@@ -2582,7 +2585,7 @@
       </c>
       <c r="K24">
         <f t="shared" si="5"/>
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="L24">
         <v>1112600</v>
@@ -2600,7 +2603,7 @@
       </c>
       <c r="P24">
         <f t="shared" si="8"/>
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
@@ -2623,7 +2626,7 @@
       </c>
       <c r="F25">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="G25">
         <v>505200</v>
@@ -2641,7 +2644,7 @@
       </c>
       <c r="K25">
         <f t="shared" si="5"/>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="L25">
         <v>496500</v>
@@ -2659,7 +2662,7 @@
       </c>
       <c r="P25">
         <f t="shared" si="8"/>
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
@@ -2682,7 +2685,7 @@
       </c>
       <c r="F26">
         <f t="shared" si="2"/>
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="G26">
         <v>5442200</v>
@@ -2700,7 +2703,7 @@
       </c>
       <c r="K26">
         <f t="shared" si="5"/>
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="L26">
         <v>5430700</v>
@@ -2718,7 +2721,7 @@
       </c>
       <c r="P26">
         <f t="shared" si="8"/>
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
@@ -2735,13 +2738,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E27" s="5" t="str">
+      <c r="E27" s="5">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F27" t="str">
+        <v>0</v>
+      </c>
+      <c r="F27">
         <f t="shared" si="2"/>
-        <v/>
+        <v>47</v>
       </c>
       <c r="G27">
         <v>0</v>
@@ -2753,13 +2756,13 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J27" s="5" t="str">
+      <c r="J27" s="5">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="K27" t="str">
+        <v>0</v>
+      </c>
+      <c r="K27">
         <f t="shared" si="5"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="L27">
         <v>0</v>
@@ -2771,13 +2774,13 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O27" s="5" t="str">
+      <c r="O27" s="5">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="P27" t="str">
+        <v>0</v>
+      </c>
+      <c r="P27">
         <f t="shared" si="8"/>
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
@@ -2800,7 +2803,7 @@
       </c>
       <c r="F28">
         <f t="shared" si="2"/>
-        <v>46</v>
+        <v>3</v>
       </c>
       <c r="G28">
         <v>1545700</v>
@@ -2818,7 +2821,7 @@
       </c>
       <c r="K28">
         <f t="shared" si="5"/>
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L28">
         <v>1525900</v>
@@ -2836,7 +2839,7 @@
       </c>
       <c r="P28">
         <f t="shared" si="8"/>
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
@@ -2859,7 +2862,7 @@
       </c>
       <c r="F29">
         <f t="shared" si="2"/>
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G29">
         <v>2779500</v>
@@ -2877,7 +2880,7 @@
       </c>
       <c r="K29">
         <f t="shared" si="5"/>
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="L29">
         <v>2889900</v>
@@ -2895,7 +2898,7 @@
       </c>
       <c r="P29">
         <f t="shared" si="8"/>
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
@@ -2918,7 +2921,7 @@
       </c>
       <c r="F30">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="G30">
         <v>12735900</v>
@@ -2936,7 +2939,7 @@
       </c>
       <c r="K30">
         <f t="shared" si="5"/>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="L30">
         <v>12861300</v>
@@ -2954,7 +2957,7 @@
       </c>
       <c r="P30">
         <f t="shared" si="8"/>
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
@@ -2977,7 +2980,7 @@
       </c>
       <c r="F31">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="G31">
         <v>1823300</v>
@@ -2995,7 +2998,7 @@
       </c>
       <c r="K31">
         <f t="shared" si="5"/>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="L31">
         <v>1870700</v>
@@ -3013,7 +3016,7 @@
       </c>
       <c r="P31">
         <f t="shared" si="8"/>
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
@@ -3036,7 +3039,7 @@
       </c>
       <c r="F32">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="G32">
         <v>6195500</v>
@@ -3054,7 +3057,7 @@
       </c>
       <c r="K32">
         <f t="shared" si="5"/>
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="L32">
         <v>6157400</v>
@@ -3072,7 +3075,7 @@
       </c>
       <c r="P32">
         <f t="shared" si="8"/>
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
@@ -3095,7 +3098,7 @@
       </c>
       <c r="F33">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G33">
         <v>979671000</v>
@@ -3113,7 +3116,7 @@
       </c>
       <c r="K33">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="L33">
         <v>989572899.99999905</v>
@@ -3131,7 +3134,7 @@
       </c>
       <c r="P33">
         <f t="shared" si="8"/>
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
@@ -3154,7 +3157,7 @@
       </c>
       <c r="F34">
         <f t="shared" si="2"/>
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G34">
         <v>4350600</v>
@@ -3172,7 +3175,7 @@
       </c>
       <c r="K34">
         <f t="shared" si="5"/>
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="L34">
         <v>4345600</v>
@@ -3190,7 +3193,7 @@
       </c>
       <c r="P34">
         <f t="shared" si="8"/>
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
@@ -3207,13 +3210,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E35" s="5" t="str">
+      <c r="E35" s="5">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F35" t="str">
+        <v>0</v>
+      </c>
+      <c r="F35">
         <f t="shared" si="2"/>
-        <v/>
+        <v>47</v>
       </c>
       <c r="G35">
         <v>0</v>
@@ -3225,13 +3228,13 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J35" s="5" t="str">
+      <c r="J35" s="5">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="K35" t="str">
+        <v>0</v>
+      </c>
+      <c r="K35">
         <f t="shared" si="5"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="L35">
         <v>0</v>
@@ -3243,13 +3246,13 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O35" s="5" t="str">
+      <c r="O35" s="5">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="P35" t="str">
+        <v>0</v>
+      </c>
+      <c r="P35">
         <f t="shared" si="8"/>
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
@@ -3272,7 +3275,7 @@
       </c>
       <c r="F36">
         <f t="shared" si="2"/>
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="G36">
         <v>898700</v>
@@ -3290,7 +3293,7 @@
       </c>
       <c r="K36">
         <f t="shared" si="5"/>
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="L36">
         <v>878300</v>
@@ -3308,7 +3311,7 @@
       </c>
       <c r="P36">
         <f t="shared" si="8"/>
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
@@ -3331,7 +3334,7 @@
       </c>
       <c r="F37">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="G37">
         <v>2229200</v>
@@ -3349,7 +3352,7 @@
       </c>
       <c r="K37">
         <f t="shared" si="5"/>
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="L37">
         <v>2296900</v>
@@ -3367,7 +3370,7 @@
       </c>
       <c r="P37">
         <f t="shared" si="8"/>
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
@@ -3390,7 +3393,7 @@
       </c>
       <c r="F38">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G38">
         <v>792800</v>
@@ -3408,7 +3411,7 @@
       </c>
       <c r="K38">
         <f t="shared" si="5"/>
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="L38">
         <v>777800</v>
@@ -3426,7 +3429,7 @@
       </c>
       <c r="P38">
         <f t="shared" si="8"/>
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
@@ -3449,7 +3452,7 @@
       </c>
       <c r="F39">
         <f t="shared" si="2"/>
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="G39">
         <v>1294400</v>
@@ -3467,7 +3470,7 @@
       </c>
       <c r="K39">
         <f t="shared" si="5"/>
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L39">
         <v>1759500</v>
@@ -3485,7 +3488,7 @@
       </c>
       <c r="P39">
         <f t="shared" si="8"/>
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
@@ -3508,7 +3511,7 @@
       </c>
       <c r="F40">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G40">
         <v>39964900</v>
@@ -3526,7 +3529,7 @@
       </c>
       <c r="K40">
         <f t="shared" si="5"/>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="L40">
         <v>40216700</v>
@@ -3544,7 +3547,7 @@
       </c>
       <c r="P40">
         <f t="shared" si="8"/>
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
@@ -3567,7 +3570,7 @@
       </c>
       <c r="F41">
         <f t="shared" si="2"/>
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="G41">
         <v>5089500</v>
@@ -3585,7 +3588,7 @@
       </c>
       <c r="K41">
         <f t="shared" si="5"/>
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L41">
         <v>4799900</v>
@@ -3603,7 +3606,7 @@
       </c>
       <c r="P41">
         <f t="shared" si="8"/>
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
@@ -3626,7 +3629,7 @@
       </c>
       <c r="F42">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="G42">
         <v>199130300</v>
@@ -3644,7 +3647,7 @@
       </c>
       <c r="K42">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="L42">
         <v>199954600</v>
@@ -3662,7 +3665,7 @@
       </c>
       <c r="P42">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
@@ -3685,7 +3688,7 @@
       </c>
       <c r="F43">
         <f t="shared" si="2"/>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G43">
         <v>8560800</v>
@@ -3703,7 +3706,7 @@
       </c>
       <c r="K43">
         <f t="shared" si="5"/>
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="L43">
         <v>8497500</v>
@@ -3721,7 +3724,7 @@
       </c>
       <c r="P43">
         <f t="shared" si="8"/>
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
@@ -3744,7 +3747,7 @@
       </c>
       <c r="F44">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="G44">
         <v>31040700</v>
@@ -3762,7 +3765,7 @@
       </c>
       <c r="K44">
         <f t="shared" si="5"/>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="L44">
         <v>31282200</v>
@@ -3780,7 +3783,7 @@
       </c>
       <c r="P44">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
@@ -3803,7 +3806,7 @@
       </c>
       <c r="F45">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="G45">
         <v>56792200</v>
@@ -3821,7 +3824,7 @@
       </c>
       <c r="K45">
         <f t="shared" si="5"/>
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L45">
         <v>56027100</v>
@@ -3839,7 +3842,7 @@
       </c>
       <c r="P45">
         <f t="shared" si="8"/>
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
@@ -3862,7 +3865,7 @@
       </c>
       <c r="F46">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="G46">
         <v>266000</v>
@@ -3880,7 +3883,7 @@
       </c>
       <c r="K46">
         <f t="shared" si="5"/>
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="L46">
         <v>267100</v>
@@ -3898,7 +3901,7 @@
       </c>
       <c r="P46">
         <f t="shared" si="8"/>
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
@@ -3921,7 +3924,7 @@
       </c>
       <c r="F47">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="G47">
         <v>73467000</v>
@@ -3939,7 +3942,7 @@
       </c>
       <c r="K47">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="L47">
         <v>75072800</v>
@@ -3957,7 +3960,7 @@
       </c>
       <c r="P47">
         <f t="shared" si="8"/>
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
@@ -3980,7 +3983,7 @@
       </c>
       <c r="F48">
         <f t="shared" si="2"/>
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="G48">
         <v>7214700</v>
@@ -3998,7 +4001,7 @@
       </c>
       <c r="K48">
         <f t="shared" si="5"/>
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="L48">
         <v>7289800</v>
@@ -4016,7 +4019,7 @@
       </c>
       <c r="P48">
         <f t="shared" si="8"/>
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
@@ -4039,7 +4042,7 @@
       </c>
       <c r="F49">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="G49">
         <v>102600</v>
@@ -4057,7 +4060,7 @@
       </c>
       <c r="K49">
         <f t="shared" si="5"/>
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="L49">
         <v>0</v>
@@ -4069,13 +4072,13 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O49" s="5" t="str">
+      <c r="O49" s="5">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="P49" t="str">
+        <v>0</v>
+      </c>
+      <c r="P49">
         <f t="shared" si="8"/>
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
@@ -4098,7 +4101,7 @@
       </c>
       <c r="F50">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>47</v>
       </c>
       <c r="G50">
         <v>859100</v>
@@ -4157,7 +4160,7 @@
       </c>
       <c r="F51">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="G51">
         <v>8925500</v>
@@ -4175,7 +4178,7 @@
       </c>
       <c r="K51">
         <f t="shared" si="5"/>
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="L51">
         <v>8833900</v>
@@ -4193,7 +4196,7 @@
       </c>
       <c r="P51">
         <f t="shared" si="8"/>
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
@@ -4216,7 +4219,7 @@
       </c>
       <c r="F52">
         <f t="shared" si="2"/>
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="G52">
         <v>2440700</v>
@@ -4234,7 +4237,7 @@
       </c>
       <c r="K52">
         <f t="shared" si="5"/>
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="L52">
         <v>2321600</v>
@@ -4252,7 +4255,7 @@
       </c>
       <c r="P52">
         <f t="shared" si="8"/>
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
@@ -4279,15 +4282,15 @@
         <v>24</v>
       </c>
       <c r="B56">
-        <f>VLOOKUP(A56,$A$2:$P$52,MATCH($B$55,$1:$1))</f>
+        <f>VLOOKUP($A56,$A$2:$P$52,MATCH(B$55,$1:$1))</f>
         <v>-36209.630000000005</v>
       </c>
       <c r="C56">
-        <f>VLOOKUP(A56,$A$2:$P$52,MATCH($C$55,$1:$1))</f>
+        <f t="shared" ref="C56:D61" si="9">VLOOKUP($A56,$A$2:$P$52,MATCH(C$55,$1:$1))</f>
         <v>-27292.159999999974</v>
       </c>
       <c r="D56">
-        <f>VLOOKUP(A56,$A$2:$P$52,MATCH($D$55,$1:$1))</f>
+        <f t="shared" si="9"/>
         <v>-9181.0800000000163</v>
       </c>
     </row>
@@ -4296,15 +4299,15 @@
         <v>25</v>
       </c>
       <c r="B57">
-        <f t="shared" ref="B57:B61" si="9">VLOOKUP(A57,$A$2:$P$52,MATCH($B$55,$1:$1))</f>
+        <f>VLOOKUP($A57,$A$2:$P$52,MATCH(B$55,$1:$1))</f>
         <v>0</v>
       </c>
       <c r="C57">
-        <f t="shared" ref="C57:C61" si="10">VLOOKUP(A57,$A$2:$P$52,MATCH($C$55,$1:$1))</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="D57">
-        <f t="shared" ref="D57:D61" si="11">VLOOKUP(A57,$A$2:$P$52,MATCH($D$55,$1:$1))</f>
+        <f t="shared" si="9"/>
         <v>-311228.08999999997</v>
       </c>
     </row>
@@ -4313,15 +4316,15 @@
         <v>32</v>
       </c>
       <c r="B58">
+        <f>VLOOKUP($A58,$A$2:$P$52,MATCH(B$55,$1:$1))</f>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="C58">
         <f t="shared" si="9"/>
-        <v>-149396.10000000987</v>
-      </c>
-      <c r="C58">
-        <f t="shared" si="10"/>
         <v>-189254.06000000006</v>
       </c>
       <c r="D58">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-374962.91000000015</v>
       </c>
     </row>
@@ -4330,15 +4333,15 @@
         <v>38</v>
       </c>
       <c r="B59">
+        <f>VLOOKUP($A59,$A$2:$P$52,MATCH(B$55,$1:$1))</f>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="C59">
         <f t="shared" si="9"/>
-        <v>-12230.810000000056</v>
-      </c>
-      <c r="C59">
-        <f t="shared" si="10"/>
         <v>-45485.580000000075</v>
       </c>
       <c r="D59">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-72.879999999888241</v>
       </c>
     </row>
@@ -4347,15 +4350,15 @@
         <v>39</v>
       </c>
       <c r="B60">
+        <f>VLOOKUP($A60,$A$2:$P$52,MATCH(B$55,$1:$1))</f>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="C60">
         <f t="shared" si="9"/>
-        <v>-4950.4699999999721</v>
-      </c>
-      <c r="C60">
-        <f t="shared" si="10"/>
         <v>-8005.7900000010268</v>
       </c>
       <c r="D60">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-1724.9000000000233</v>
       </c>
     </row>
@@ -4364,15 +4367,15 @@
         <v>55</v>
       </c>
       <c r="B61">
+        <f>VLOOKUP($A61,$A$2:$P$52,MATCH(B$55,$1:$1))</f>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="C61">
         <f t="shared" si="9"/>
-        <v>-184239.79000001028</v>
-      </c>
-      <c r="C61">
-        <f t="shared" si="10"/>
         <v>-133456.33000001032</v>
       </c>
       <c r="D61">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-82077.349999999627</v>
       </c>
     </row>
@@ -4394,180 +4397,235 @@
       <c r="D64" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F64" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>24</v>
       </c>
       <c r="B65">
-        <f>_xlfn.XLOOKUP(A65,$A$2:$A$52,$D$2:$D$52)</f>
+        <f t="shared" ref="B65:B70" si="10">_xlfn.XLOOKUP(A65,$A$2:$A$52,$D$2:$D$52)</f>
         <v>-36209.630000000005</v>
       </c>
       <c r="C65">
-        <f>_xlfn.XLOOKUP(A65,$A$2:$A$52,$I$2:$I$52)</f>
+        <f t="shared" ref="C65:C70" si="11">_xlfn.XLOOKUP(A65,$A$2:$A$52,$I$2:$I$52)</f>
         <v>-27292.159999999974</v>
       </c>
       <c r="D65">
         <f>_xlfn.XLOOKUP(A65,$A$2:$A$52,$N$2:$N$52)</f>
         <v>-9181.0800000000163</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F65" t="e">
+        <f>_xlfn.XLOOKUP($A65,$A$1:$A$52,INDEX($A$1:$P$52,MATCH(B$64,$1:$1,0)),FALSE)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>25</v>
       </c>
       <c r="B66">
-        <f t="shared" ref="B66:B70" si="12">_xlfn.XLOOKUP(A66,$A$2:$A$52,$D$2:$D$52)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="C66">
-        <f t="shared" ref="C66:C70" si="13">_xlfn.XLOOKUP(A66,$A$2:$A$52,$I$2:$I$52)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="D66">
-        <f t="shared" ref="D66:D70" si="14">_xlfn.XLOOKUP(A66,$A$2:$A$52,$N$2:$N$52)</f>
+        <f t="shared" ref="D66:D70" si="12">_xlfn.XLOOKUP(A66,$A$2:$A$52,$N$2:$N$52)</f>
         <v>-311228.08999999997</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>32</v>
       </c>
       <c r="B67">
+        <f t="shared" si="10"/>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="C67">
+        <f t="shared" si="11"/>
+        <v>-189254.06000000006</v>
+      </c>
+      <c r="D67">
         <f t="shared" si="12"/>
+        <v>-374962.91000000015</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>38</v>
+      </c>
+      <c r="B68">
+        <f t="shared" si="10"/>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="C68">
+        <f t="shared" si="11"/>
+        <v>-45485.580000000075</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="12"/>
+        <v>-72.879999999888241</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>39</v>
+      </c>
+      <c r="B69">
+        <f t="shared" si="10"/>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="C69">
+        <f t="shared" si="11"/>
+        <v>-8005.7900000010268</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="12"/>
+        <v>-1724.9000000000233</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>55</v>
+      </c>
+      <c r="B70">
+        <f t="shared" si="10"/>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="C70">
+        <f t="shared" si="11"/>
+        <v>-133456.33000001032</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="12"/>
+        <v>-82077.349999999627</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>24</v>
+      </c>
+      <c r="B74">
+        <f>INDEX($A$1:$P$52,MATCH($A74,$A$1:$A$52,0),MATCH(B$73,$A$1:$P$1,0))</f>
+        <v>-36209.630000000005</v>
+      </c>
+      <c r="C74">
+        <f>INDEX($A$1:$P$52,MATCH($A74,$A$1:$A$52,0),MATCH(C$73,$A$1:$P$1,0))</f>
+        <v>-27292.159999999974</v>
+      </c>
+      <c r="D74">
+        <f>INDEX($A$1:$P$52,MATCH($A74,$A$1:$A$52,0),MATCH(D$73,$A$1:$P$1,0))</f>
+        <v>-9181.0800000000163</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>25</v>
+      </c>
+      <c r="B75">
+        <f t="shared" ref="B75:D79" si="13">INDEX($A$1:$P$52,MATCH($A75,$A$1:$A$52,0),MATCH(B$73,$A$1:$P$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="C75">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <f t="shared" si="13"/>
+        <v>-311228.08999999997</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>32</v>
+      </c>
+      <c r="B76">
+        <f t="shared" si="13"/>
         <v>-149396.10000000987</v>
       </c>
-      <c r="C67">
+      <c r="C76">
         <f t="shared" si="13"/>
         <v>-189254.06000000006</v>
       </c>
-      <c r="D67">
-        <f t="shared" si="14"/>
+      <c r="D76">
+        <f t="shared" si="13"/>
         <v>-374962.91000000015</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>38</v>
       </c>
-      <c r="B68">
-        <f t="shared" si="12"/>
+      <c r="B77">
+        <f t="shared" si="13"/>
         <v>-12230.810000000056</v>
       </c>
-      <c r="C68">
+      <c r="C77">
         <f t="shared" si="13"/>
         <v>-45485.580000000075</v>
       </c>
-      <c r="D68">
-        <f t="shared" si="14"/>
+      <c r="D77">
+        <f t="shared" si="13"/>
         <v>-72.879999999888241</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>39</v>
       </c>
-      <c r="B69">
-        <f t="shared" si="12"/>
+      <c r="B78">
+        <f>INDEX($A$1:$P$52,MATCH($A78,$A$1:$A$52,0),MATCH(B$73,$A$1:$P$1,0))</f>
         <v>-4950.4699999999721</v>
       </c>
-      <c r="C69">
+      <c r="C78">
+        <f>INDEX($A$1:$P$52,MATCH($A78,$A$1:$A$52,0),MATCH(C$73,$A$1:$P$1,0))</f>
+        <v>-8005.7900000010268</v>
+      </c>
+      <c r="D78">
+        <f>INDEX($A$1:$P$52,MATCH($A78,$A$1:$A$52,0),MATCH(D$73,$A$1:$P$1,0))</f>
+        <v>-1724.9000000000233</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>55</v>
+      </c>
+      <c r="B79">
         <f t="shared" si="13"/>
-        <v>-8005.7900000010268</v>
-      </c>
-      <c r="D69">
-        <f t="shared" si="14"/>
-        <v>-1724.9000000000233</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>55</v>
-      </c>
-      <c r="B70">
-        <f t="shared" si="12"/>
         <v>-184239.79000001028</v>
       </c>
-      <c r="C70">
+      <c r="C79">
         <f t="shared" si="13"/>
         <v>-133456.33000001032</v>
       </c>
-      <c r="D70">
-        <f t="shared" si="14"/>
+      <c r="D79">
+        <f t="shared" si="13"/>
         <v>-82077.349999999627</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>24</v>
-      </c>
-      <c r="B74">
-        <f>INDEX($A$2:$P$52,MATCH(A74,$A$2:$A$52,0),MATCH(B73,$1:$1,0))</f>
-        <v>-36209.630000000005</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>25</v>
-      </c>
-      <c r="B75" t="e">
-        <f>INDEX($A$2:$P$52,MATCH(A75,$A$2:$A$52,0),MATCH(B74,$1:$1,0))</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>32</v>
-      </c>
-      <c r="B76" t="e">
-        <f t="shared" ref="B75:B79" si="15">INDEX($A$2:$P$52,MATCH(A76,$A$2:$A$52,0),MATCH(B75,$1:$1,0))</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>38</v>
-      </c>
-      <c r="B77" t="e">
-        <f t="shared" si="15"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>39</v>
-      </c>
-      <c r="B78" t="e">
-        <f t="shared" si="15"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>55</v>
-      </c>
-      <c r="B79" t="e">
-        <f t="shared" si="15"/>
-        <v>#N/A</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -4579,6 +4637,9 @@
       <c r="A82" t="s">
         <v>0</v>
       </c>
+      <c r="B82" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B83" s="1" t="s">
@@ -4592,7 +4653,10 @@
       <c r="A84" t="s">
         <v>73</v>
       </c>
-      <c r="B84" s="6"/>
+      <c r="B84" t="e">
+        <f>INDEX($A$2:$P$52,MATCH(B87,$A$2:$A$52,0),MATCH($B$83,$1:$1,0))</f>
+        <v>#N/A</v>
+      </c>
       <c r="C84" s="6"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -4608,6 +4672,11 @@
       </c>
       <c r="B86" s="6"/>
       <c r="C86" s="6"/>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
@@ -4743,11 +4812,14 @@
       <c r="I100" s="4"/>
     </row>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A83" xr:uid="{0ECE0BAD-DC74-4E7B-8842-0609702F3664}">
       <formula1>$A$2:$A$52</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B82:B83" xr:uid="{1248789C-8354-428B-8B98-C97B02054C67}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B87" xr:uid="{7D422295-6758-4769-85D3-20041286AFD1}">
+      <formula1>A2:A52</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>